<commit_message>
student details have been added
Added support for more student details, started with GUI
</commit_message>
<xml_diff>
--- a/Attendance.xlsx
+++ b/Attendance.xlsx
@@ -1,120 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Student details" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="18">
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Roll no</t>
-  </si>
-  <si>
-    <t>2023-01-15</t>
-  </si>
-  <si>
-    <t>2023-01-16</t>
-  </si>
-  <si>
-    <t>2023-02-01</t>
-  </si>
-  <si>
-    <t>2023-02-08</t>
-  </si>
-  <si>
-    <t>2023-02-09</t>
-  </si>
-  <si>
-    <t>2023-03-12</t>
-  </si>
-  <si>
-    <t>Manraj Singh</t>
-  </si>
-  <si>
-    <t>In-time: 08:49:41 Out-time: 15:12:12</t>
-  </si>
-  <si>
-    <t>In-time: 08:53:31 Out-time: 14:32:12</t>
-  </si>
-  <si>
-    <t>In-time: 08:29:14 
-Out-time: 15:15:56</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>In-time: 09:00:03 
-Out-time: 12:12:12</t>
-  </si>
-  <si>
-    <t>Arya</t>
-  </si>
-  <si>
-    <t>Bipin</t>
-  </si>
-  <si>
-    <t>In-time: 16:53:57</t>
-  </si>
-  <si>
-    <t>In-time: 16:53:58 
-Out-time: 16:54:15</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -126,52 +46,90 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -459,128 +417,132 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
+    <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" style="9" width="15.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="11" width="17.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="11" width="17.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="11" width="19.005" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="11" width="17.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="11" width="20.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="3" min="1" max="1"/>
+    <col width="15.86214285714286" bestFit="1" customWidth="1" style="3" min="2" max="2"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>7</v>
+    <row r="1" ht="18.75" customHeight="1">
+      <c r="A1" s="3" t="inlineStr">
+        <is>
+          <t>Roll number</t>
+        </is>
+      </c>
+      <c r="B1" s="3" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>2023-03-12</t>
+        </is>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="46.5">
-      <c r="A2" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="6">
-        <v>69</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>12</v>
+    <row r="2" ht="18.75" customHeight="1">
+      <c r="A2" s="2" t="n">
+        <v>72</v>
+      </c>
+      <c r="B2" s="3" t="inlineStr">
+        <is>
+          <t>Piyush Chugeja</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>In-time: 19:52:10 
+Out-time: 19:52:25</t>
+        </is>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
-      <c r="A3" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="8">
-        <v>27</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>12</v>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="3" min="1" max="1"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="3" min="2" max="2"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="3" min="3" max="3"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="3" min="4" max="4"/>
+    <col width="19.86214285714286" bestFit="1" customWidth="1" style="3" min="5" max="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="18.75" customHeight="1">
+      <c r="A1" s="3" t="inlineStr">
+        <is>
+          <t>Roll number</t>
+        </is>
+      </c>
+      <c r="B1" s="3" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="C1" s="3" t="inlineStr">
+        <is>
+          <t>Phone number</t>
+        </is>
+      </c>
+      <c r="D1" s="3" t="inlineStr">
+        <is>
+          <t>Parent name</t>
+        </is>
+      </c>
+      <c r="E1" s="3" t="inlineStr">
+        <is>
+          <t>Parent phone number</t>
+        </is>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="31.5">
-      <c r="A4" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="8">
-        <v>31</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>17</v>
+    <row r="2" ht="18.75" customHeight="1">
+      <c r="A2" s="3" t="inlineStr">
+        <is>
+          <t>72</t>
+        </is>
+      </c>
+      <c r="B2" s="3" t="inlineStr">
+        <is>
+          <t>Piyush Chugeja</t>
+        </is>
+      </c>
+      <c r="C2" s="2" t="n">
+        <v>7506699134</v>
+      </c>
+      <c r="D2" s="3" t="inlineStr">
+        <is>
+          <t>Muskan</t>
+        </is>
+      </c>
+      <c r="E2" s="3" t="inlineStr">
+        <is>
+          <t>9821539523</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new sheet created for each month
</commit_message>
<xml_diff>
--- a/Attendance.xlsx
+++ b/Attendance.xlsx
@@ -3,11 +3,11 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Student details" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Student details" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="March" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -17,13 +17,25 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color rgb="FF000000"/>
+      <sz val="11"/>
     </font>
   </fonts>
   <fills count="2">
@@ -34,7 +46,14 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left/>
       <right/>
@@ -44,18 +63,27 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general"/>
     </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general"/>
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -422,48 +450,70 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="3" min="1" max="1"/>
-    <col width="15.86214285714286" bestFit="1" customWidth="1" style="3" min="2" max="2"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="4" min="1" max="1"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="5" min="2" max="2"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="5" min="3" max="3"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="5" min="4" max="4"/>
+    <col width="19.86214285714286" bestFit="1" customWidth="1" style="5" min="5" max="5"/>
   </cols>
   <sheetData>
-    <row r="1" ht="18.75" customHeight="1">
+    <row r="1" ht="19.5" customHeight="1">
       <c r="A1" s="3" t="inlineStr">
         <is>
           <t>Roll number</t>
         </is>
       </c>
-      <c r="B1" s="3" t="inlineStr">
+      <c r="B1" s="5" t="inlineStr">
         <is>
           <t>Name</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>2023-03-12</t>
+      <c r="C1" s="6" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+      <c r="D1" s="5" t="inlineStr">
+        <is>
+          <t>Parent name</t>
+        </is>
+      </c>
+      <c r="E1" s="5" t="inlineStr">
+        <is>
+          <t>Parent email</t>
         </is>
       </c>
     </row>
     <row r="2" ht="18.75" customHeight="1">
-      <c r="A2" s="2" t="n">
+      <c r="A2" s="3" t="n">
         <v>72</v>
       </c>
-      <c r="B2" s="3" t="inlineStr">
+      <c r="B2" s="5" t="inlineStr">
         <is>
           <t>Piyush Chugeja</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>In-time: 19:52:10 
-Out-time: 19:52:25</t>
+      <c r="C2" s="5" t="inlineStr">
+        <is>
+          <t>piyushchugeja@gmail.com</t>
+        </is>
+      </c>
+      <c r="D2" s="5" t="inlineStr">
+        <is>
+          <t>Muskan</t>
+        </is>
+      </c>
+      <c r="E2" s="5" t="inlineStr">
+        <is>
+          <t>muskan.chugeja@gmail.com</t>
         </is>
       </c>
     </row>
@@ -478,70 +528,49 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="3" min="1" max="1"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="3" min="2" max="2"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="3" min="3" max="3"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="3" min="4" max="4"/>
-    <col width="19.86214285714286" bestFit="1" customWidth="1" style="3" min="5" max="5"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="4" min="1" max="1"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="5" min="2" max="2"/>
+    <col width="17.14785714285714" bestFit="1" customWidth="1" style="5" min="3" max="3"/>
   </cols>
   <sheetData>
     <row r="1" ht="18.75" customHeight="1">
-      <c r="A1" s="3" t="inlineStr">
-        <is>
-          <t>Roll number</t>
-        </is>
-      </c>
-      <c r="B1" s="3" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Roll no</t>
+        </is>
+      </c>
+      <c r="B1" s="5" t="inlineStr">
         <is>
           <t>Name</t>
         </is>
       </c>
-      <c r="C1" s="3" t="inlineStr">
-        <is>
-          <t>Phone number</t>
-        </is>
-      </c>
-      <c r="D1" s="3" t="inlineStr">
-        <is>
-          <t>Parent name</t>
-        </is>
-      </c>
-      <c r="E1" s="3" t="inlineStr">
-        <is>
-          <t>Parent phone number</t>
+      <c r="C1" s="5" t="inlineStr">
+        <is>
+          <t>2023-03-12</t>
         </is>
       </c>
     </row>
-    <row r="2" ht="18.75" customHeight="1">
-      <c r="A2" s="3" t="inlineStr">
-        <is>
-          <t>72</t>
-        </is>
-      </c>
-      <c r="B2" s="3" t="inlineStr">
+    <row r="2" ht="31.5" customHeight="1">
+      <c r="A2" s="3" t="n">
+        <v>72</v>
+      </c>
+      <c r="B2" s="5" t="inlineStr">
         <is>
           <t>Piyush Chugeja</t>
         </is>
       </c>
-      <c r="C2" s="2" t="n">
-        <v>7506699134</v>
-      </c>
-      <c r="D2" s="3" t="inlineStr">
-        <is>
-          <t>Muskan</t>
-        </is>
-      </c>
-      <c r="E2" s="3" t="inlineStr">
-        <is>
-          <t>9821539523</t>
+      <c r="C2" s="5" t="inlineStr">
+        <is>
+          <t>In-time: 23:57:54 
+Out-time: 23:57:56</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed a tiny updation mistake
The wrong column number was being returned by the `add_column` method.
</commit_message>
<xml_diff>
--- a/Attendance.xlsx
+++ b/Attendance.xlsx
@@ -17,19 +17,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -65,7 +59,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
@@ -73,16 +67,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -458,60 +449,60 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="4" min="1" max="1"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="5" min="2" max="2"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="5" min="3" max="3"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="5" min="4" max="4"/>
-    <col width="19.86214285714286" bestFit="1" customWidth="1" style="5" min="5" max="5"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="3" min="1" max="1"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="4" min="2" max="2"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="4" min="3" max="3"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="4" min="4" max="4"/>
+    <col width="19.86214285714286" bestFit="1" customWidth="1" style="4" min="5" max="5"/>
   </cols>
   <sheetData>
     <row r="1" ht="19.5" customHeight="1">
-      <c r="A1" s="3" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Roll number</t>
         </is>
       </c>
-      <c r="B1" s="5" t="inlineStr">
+      <c r="B1" s="4" t="inlineStr">
         <is>
           <t>Name</t>
         </is>
       </c>
-      <c r="C1" s="6" t="inlineStr">
+      <c r="C1" s="5" t="inlineStr">
         <is>
           <t>Email</t>
         </is>
       </c>
-      <c r="D1" s="5" t="inlineStr">
+      <c r="D1" s="4" t="inlineStr">
         <is>
           <t>Parent name</t>
         </is>
       </c>
-      <c r="E1" s="5" t="inlineStr">
+      <c r="E1" s="4" t="inlineStr">
         <is>
           <t>Parent email</t>
         </is>
       </c>
     </row>
     <row r="2" ht="18.75" customHeight="1">
-      <c r="A2" s="3" t="n">
+      <c r="A2" s="1" t="n">
         <v>72</v>
       </c>
-      <c r="B2" s="5" t="inlineStr">
+      <c r="B2" s="4" t="inlineStr">
         <is>
           <t>Piyush Chugeja</t>
         </is>
       </c>
-      <c r="C2" s="5" t="inlineStr">
+      <c r="C2" s="4" t="inlineStr">
         <is>
           <t>piyushchugeja@gmail.com</t>
         </is>
       </c>
-      <c r="D2" s="5" t="inlineStr">
+      <c r="D2" s="4" t="inlineStr">
         <is>
           <t>Muskan</t>
         </is>
       </c>
-      <c r="E2" s="5" t="inlineStr">
+      <c r="E2" s="4" t="inlineStr">
         <is>
           <t>muskan.chugeja@gmail.com</t>
         </is>
@@ -528,7 +519,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -536,41 +527,52 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="4" min="1" max="1"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="5" min="2" max="2"/>
-    <col width="17.14785714285714" bestFit="1" customWidth="1" style="5" min="3" max="3"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="3" min="1" max="1"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="4" min="2" max="2"/>
+    <col width="17.14785714285714" bestFit="1" customWidth="1" style="4" min="3" max="3"/>
   </cols>
   <sheetData>
-    <row r="1" ht="18.75" customHeight="1">
+    <row r="1" ht="19.5" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Roll no</t>
         </is>
       </c>
-      <c r="B1" s="5" t="inlineStr">
+      <c r="B1" s="4" t="inlineStr">
         <is>
           <t>Name</t>
         </is>
       </c>
-      <c r="C1" s="5" t="inlineStr">
+      <c r="C1" s="4" t="inlineStr">
         <is>
           <t>2023-03-12</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>2023-03-13</t>
         </is>
       </c>
     </row>
     <row r="2" ht="31.5" customHeight="1">
-      <c r="A2" s="3" t="n">
+      <c r="A2" s="1" t="n">
         <v>72</v>
       </c>
-      <c r="B2" s="5" t="inlineStr">
+      <c r="B2" s="4" t="inlineStr">
         <is>
           <t>Piyush Chugeja</t>
         </is>
       </c>
-      <c r="C2" s="5" t="inlineStr">
+      <c r="C2" s="4" t="inlineStr">
         <is>
           <t>In-time: 23:57:54 
 Out-time: 23:57:56</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>In-time: 00:04:45 
+Out-time: 00:04:49</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
added user deletion and picture click
</commit_message>
<xml_diff>
--- a/Attendance.xlsx
+++ b/Attendance.xlsx
@@ -541,91 +541,95 @@
     </row>
     <row r="2" ht="19.5" customHeight="1">
       <c r="A2" s="1" t="n">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B2" s="12" t="inlineStr">
         <is>
-          <t>Piyush</t>
-        </is>
-      </c>
-      <c r="C2" s="15" t="inlineStr">
-        <is>
-          <t>d2021.piyush.chugeja@ves.ac.in</t>
+          <t>Manraj</t>
+        </is>
+      </c>
+      <c r="C2" s="16" t="inlineStr">
+        <is>
+          <t>d2021.manrajsingh.virdi@ves.ac.in</t>
         </is>
       </c>
       <c r="D2" s="1" t="n">
-        <v>7506699134</v>
-      </c>
-      <c r="E2" s="14" t="n">
-        <v>25569.22946260417</v>
+        <v>8424036665</v>
+      </c>
+      <c r="E2" s="17" t="inlineStr">
+        <is>
+          <t>29/12/2003</t>
+        </is>
       </c>
     </row>
     <row r="3" ht="19.5" customHeight="1">
       <c r="A3" s="1" t="n">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B3" s="12" t="inlineStr">
         <is>
-          <t>Manraj</t>
+          <t>Sakshi</t>
         </is>
       </c>
       <c r="C3" s="16" t="inlineStr">
         <is>
-          <t>d2021.manrajsingh.virdi@ves.ac.in</t>
+          <t>d2021.sakshi.kirmathe@ves.ac.in</t>
         </is>
       </c>
       <c r="D3" s="1" t="n">
-        <v>8424036665</v>
-      </c>
-      <c r="E3" s="17" t="inlineStr">
-        <is>
-          <t>29/12/2003</t>
-        </is>
+        <v>8652839845</v>
+      </c>
+      <c r="E3" s="17" t="n">
+        <v>25569.22946260417</v>
       </c>
     </row>
     <row r="4" ht="19.5" customHeight="1">
-      <c r="A4" s="1" t="n">
-        <v>71</v>
-      </c>
-      <c r="B4" s="12" t="inlineStr">
-        <is>
-          <t>Sakshi</t>
-        </is>
-      </c>
-      <c r="C4" s="16" t="inlineStr">
-        <is>
-          <t>d2021.sakshi.kirmathe@ves.ac.in</t>
-        </is>
-      </c>
-      <c r="D4" s="1" t="n">
-        <v>8652839845</v>
-      </c>
-      <c r="E4" s="17" t="n">
-        <v>25569.22946260417</v>
+      <c r="A4" t="n">
+        <v>39</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Nitesh</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>dsds@gmas.d</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>8779340262</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>04/07/2009</t>
+        </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>39</v>
+        <v>72</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Nitesh</t>
+          <t>Piyush Chugeja</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>dsds@gmas.d</t>
+          <t>d2021.piyush.chugeja@ves.ac.in</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>8779340262</t>
+          <t>7506699134</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>04/07/2009</t>
+          <t>02/12/2003</t>
         </is>
       </c>
     </row>
@@ -672,45 +676,45 @@
     </row>
     <row r="2" ht="18.75" customHeight="1">
       <c r="A2" s="1" t="n">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B2" s="12" t="inlineStr">
         <is>
-          <t>Piyush Chugeja</t>
+          <t>Manraj</t>
         </is>
       </c>
       <c r="C2" s="3" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>In-time: 08:43:19 
+Out-time: 15:43:54</t>
         </is>
       </c>
     </row>
     <row r="3" ht="18.75" customHeight="1">
       <c r="A3" s="1" t="n">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B3" s="12" t="inlineStr">
         <is>
-          <t>Manraj</t>
+          <t>Sakshi</t>
         </is>
       </c>
       <c r="C3" s="3" t="inlineStr">
         <is>
-          <t>In-time: 08:43:19 
-Out-time: 15:43:54</t>
+          <t>A</t>
         </is>
       </c>
     </row>
     <row r="4" ht="18.75" customHeight="1">
-      <c r="A4" s="1" t="n">
-        <v>71</v>
-      </c>
-      <c r="B4" s="12" t="inlineStr">
-        <is>
-          <t>Sakshi</t>
-        </is>
-      </c>
-      <c r="C4" s="3" t="inlineStr">
+      <c r="A4" t="n">
+        <v>39</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Nitesh</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
         <is>
           <t>A</t>
         </is>
@@ -718,11 +722,11 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>39</v>
+        <v>72</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Nitesh</t>
+          <t>Piyush Chugeja</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -786,46 +790,44 @@
     </row>
     <row r="2" ht="60" customHeight="1">
       <c r="A2" s="5" t="n">
-        <v>72</v>
-      </c>
-      <c r="B2" s="6" t="inlineStr">
-        <is>
-          <t>Piyush</t>
-        </is>
-      </c>
-      <c r="C2" s="7" t="inlineStr">
-        <is>
-          <t>A</t>
+        <v>69</v>
+      </c>
+      <c r="B2" s="12" t="inlineStr">
+        <is>
+          <t>Manraj</t>
+        </is>
+      </c>
+      <c r="C2" s="8" t="inlineStr">
+        <is>
+          <t>In-time: 08:43:19 Out-time: 15:43:54</t>
         </is>
       </c>
       <c r="D2" s="3" t="inlineStr">
         <is>
-          <t>In-time: 22:31:49 
-Out-time: 22:32:01</t>
+          <t>A</t>
         </is>
       </c>
       <c r="E2" s="3" t="inlineStr">
         <is>
-          <t>In-time: 02:12:12 
-Out-time: 03:30:47</t>
+          <t>A</t>
         </is>
       </c>
     </row>
     <row r="3" ht="46.5" customHeight="1">
-      <c r="A3" s="5" t="n">
-        <v>69</v>
-      </c>
-      <c r="B3" s="12" t="inlineStr">
-        <is>
-          <t>Manraj</t>
-        </is>
-      </c>
-      <c r="C3" s="8" t="inlineStr">
-        <is>
-          <t>In-time: 08:43:19 Out-time: 15:43:54</t>
-        </is>
-      </c>
-      <c r="D3" s="3" t="inlineStr">
+      <c r="A3" s="10" t="n">
+        <v>71</v>
+      </c>
+      <c r="B3" s="13" t="inlineStr">
+        <is>
+          <t>Sakshi</t>
+        </is>
+      </c>
+      <c r="C3" s="7" t="inlineStr">
+        <is>
+          <t>In-time: 08:52:16 Out-time: 13:43:54</t>
+        </is>
+      </c>
+      <c r="D3" s="13" t="inlineStr">
         <is>
           <t>A</t>
         </is>
@@ -837,37 +839,38 @@
       </c>
     </row>
     <row r="4" ht="44.25" customFormat="1" customHeight="1" s="9">
-      <c r="A4" s="10" t="n">
-        <v>71</v>
-      </c>
-      <c r="B4" s="13" t="inlineStr">
-        <is>
-          <t>Sakshi</t>
-        </is>
-      </c>
-      <c r="C4" s="7" t="inlineStr">
-        <is>
-          <t>In-time: 08:52:16 Out-time: 13:43:54</t>
-        </is>
-      </c>
-      <c r="D4" s="13" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="E4" s="3" t="inlineStr">
-        <is>
-          <t>A</t>
+      <c r="A4" t="n">
+        <v>39</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Nitesh</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>In-time: 03:30:29 
+Out-time: 13:45:49</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>39</v>
+        <v>72</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Nitesh</t>
+          <t>Piyush Chugeja</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -882,8 +885,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>In-time: 03:30:29 
-Out-time: 03:30:44</t>
+          <t>A</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
save the cleaner version
</commit_message>
<xml_diff>
--- a/Attendance.xlsx
+++ b/Attendance.xlsx
@@ -18,7 +18,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -30,6 +30,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <color rgb="FF000000"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color theme="1"/>
       <sz val="11"/>
     </font>
   </fonts>
@@ -60,7 +66,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
@@ -71,11 +77,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general"/>
     </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" wrapText="1"/>
+    </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment horizontal="general" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general"/>
@@ -93,7 +105,10 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left"/>
+      <alignment horizontal="general"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -460,7 +475,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,136 +483,186 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="12.14785714285714" bestFit="1" customWidth="1" style="4" min="1" max="1"/>
-    <col width="14.57642857142857" bestFit="1" customWidth="1" style="6" min="2" max="2"/>
-    <col width="30.29071428571428" bestFit="1" customWidth="1" style="6" min="3" max="3"/>
-    <col width="14.29071428571429" bestFit="1" customWidth="1" style="6" min="4" max="4"/>
-    <col width="10.71928571428571" bestFit="1" customWidth="1" style="11" min="5" max="5"/>
+    <col width="12.14785714285714" bestFit="1" customWidth="1" style="6" min="1" max="1"/>
+    <col width="14.57642857142857" bestFit="1" customWidth="1" style="8" min="2" max="2"/>
+    <col width="30.29071428571428" bestFit="1" customWidth="1" style="8" min="3" max="3"/>
+    <col width="14.29071428571429" bestFit="1" customWidth="1" style="8" min="4" max="4"/>
+    <col width="12.29071428571429" bestFit="1" customWidth="1" style="14" min="5" max="5"/>
   </cols>
   <sheetData>
     <row r="1" ht="19.5" customHeight="1">
-      <c r="A1" s="7" t="inlineStr">
+      <c r="A1" s="9" t="inlineStr">
         <is>
           <t>Employee ID</t>
         </is>
       </c>
-      <c r="B1" s="8" t="inlineStr">
+      <c r="B1" s="10" t="inlineStr">
         <is>
           <t>Name</t>
         </is>
       </c>
-      <c r="C1" s="8" t="inlineStr">
+      <c r="C1" s="10" t="inlineStr">
         <is>
           <t>Email</t>
         </is>
       </c>
-      <c r="D1" s="8" t="inlineStr">
+      <c r="D1" s="10" t="inlineStr">
         <is>
           <t>Phone number</t>
         </is>
       </c>
-      <c r="E1" s="9" t="inlineStr">
+      <c r="E1" s="11" t="inlineStr">
         <is>
           <t>DOB</t>
         </is>
       </c>
     </row>
-    <row r="2" ht="18.75" customHeight="1">
+    <row r="2" ht="19.5" customHeight="1">
       <c r="A2" s="1" t="n">
+        <v>68</v>
+      </c>
+      <c r="B2" s="8" t="inlineStr">
+        <is>
+          <t>Deven</t>
+        </is>
+      </c>
+      <c r="C2" s="8" t="inlineStr">
+        <is>
+          <t>d2021.deven.bhagtani@ves.ac.in</t>
+        </is>
+      </c>
+      <c r="D2" s="8" t="inlineStr">
+        <is>
+          <t>7218572159</t>
+        </is>
+      </c>
+      <c r="E2" s="12" t="inlineStr">
+        <is>
+          <t>10/10/2003</t>
+        </is>
+      </c>
+    </row>
+    <row r="3" ht="19.5" customHeight="1">
+      <c r="A3" s="1" t="n">
+        <v>69</v>
+      </c>
+      <c r="B3" s="8" t="inlineStr">
+        <is>
+          <t>Manraj</t>
+        </is>
+      </c>
+      <c r="C3" s="8" t="inlineStr">
+        <is>
+          <t>d2021.manrajsingh.virdi@ves.ac.in</t>
+        </is>
+      </c>
+      <c r="D3" s="8" t="inlineStr">
+        <is>
+          <t>8424036665</t>
+        </is>
+      </c>
+      <c r="E3" s="12" t="inlineStr">
+        <is>
+          <t>29/12/2003</t>
+        </is>
+      </c>
+    </row>
+    <row r="4" ht="19.5" customHeight="1">
+      <c r="A4" s="1" t="n">
+        <v>71</v>
+      </c>
+      <c r="B4" s="8" t="inlineStr">
+        <is>
+          <t>Sakshi</t>
+        </is>
+      </c>
+      <c r="C4" s="8" t="inlineStr">
+        <is>
+          <t>d2021.sakshi.kirmathe@ves.ac.in</t>
+        </is>
+      </c>
+      <c r="D4" s="8" t="inlineStr">
+        <is>
+          <t>8652839845</t>
+        </is>
+      </c>
+      <c r="E4" s="12" t="n">
+        <v>25569.22960430555</v>
+      </c>
+    </row>
+    <row r="5" ht="18.75" customHeight="1">
+      <c r="A5" s="4" t="n">
         <v>72</v>
       </c>
-      <c r="B2" s="6" t="inlineStr">
+      <c r="B5" s="8" t="inlineStr">
         <is>
           <t>Piyush</t>
         </is>
       </c>
-      <c r="C2" s="6" t="inlineStr">
-        <is>
-          <t>d2021.piyush.chugeja@ves.ac.in</t>
-        </is>
-      </c>
-      <c r="D2" s="6" t="inlineStr">
+      <c r="C5" s="8" t="inlineStr">
+        <is>
+          <t>piyushchugeja@gmail.com</t>
+        </is>
+      </c>
+      <c r="D5" s="8" t="inlineStr">
         <is>
           <t>7506699134</t>
         </is>
       </c>
-      <c r="E2" s="10" t="inlineStr">
-        <is>
-          <t>02/12/2003</t>
-        </is>
-      </c>
-    </row>
-    <row r="3" ht="18.75" customHeight="1">
-      <c r="A3" s="1" t="n">
-        <v>68</v>
-      </c>
-      <c r="B3" s="6" t="inlineStr">
-        <is>
-          <t>Deven</t>
-        </is>
-      </c>
-      <c r="C3" s="6" t="inlineStr">
-        <is>
-          <t>d2021.deven.bhagtani@ves.ac.in</t>
-        </is>
-      </c>
-      <c r="D3" s="6" t="inlineStr">
-        <is>
-          <t>7218572159</t>
-        </is>
-      </c>
-      <c r="E3" s="10" t="inlineStr">
-        <is>
-          <t>10/10/2003</t>
-        </is>
-      </c>
-    </row>
-    <row r="4" ht="18.75" customHeight="1">
-      <c r="A4" s="1" t="n">
-        <v>69</v>
-      </c>
-      <c r="B4" s="6" t="inlineStr">
-        <is>
-          <t>Manraj</t>
-        </is>
-      </c>
-      <c r="C4" s="6" t="inlineStr">
-        <is>
-          <t>d2021.manrajsingh.virdi@ves.ac.in</t>
-        </is>
-      </c>
-      <c r="D4" s="6" t="inlineStr">
-        <is>
-          <t>8424036665</t>
-        </is>
-      </c>
-      <c r="E4" s="10" t="inlineStr">
-        <is>
-          <t>29/12/2003</t>
-        </is>
-      </c>
-    </row>
-    <row r="5" ht="18.75" customHeight="1">
-      <c r="A5" s="1" t="n">
-        <v>71</v>
-      </c>
-      <c r="B5" s="6" t="inlineStr">
-        <is>
-          <t>Sakshi</t>
-        </is>
-      </c>
-      <c r="C5" s="6" t="inlineStr">
-        <is>
-          <t>d2021.sakshi.kirmathe@ves.ac.in</t>
-        </is>
-      </c>
-      <c r="D5" s="6" t="inlineStr">
-        <is>
-          <t>8652839845</t>
-        </is>
-      </c>
-      <c r="E5" s="10" t="n">
-        <v>37812</v>
+      <c r="E5" s="14" t="inlineStr">
+        <is>
+          <t>01/12/2003</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>73</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Divyaa</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>dthaivalappil@gmail.com</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>9967550586</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>01/02/2004</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>74</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Arya</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>arya232004@gmail.com</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>9004697366</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>23/01/2004</t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -611,7 +676,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -619,59 +684,79 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="4" min="1" max="1"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="6" min="2" max="2"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="6" min="1" max="1"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="8" min="2" max="2"/>
   </cols>
   <sheetData>
-    <row r="1" ht="18.75" customHeight="1">
+    <row r="1" ht="19.5" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Roll no</t>
         </is>
       </c>
-      <c r="B1" s="6" t="inlineStr">
+      <c r="B1" s="8" t="inlineStr">
         <is>
           <t>Name</t>
         </is>
       </c>
     </row>
-    <row r="2" ht="18.75" customHeight="1">
+    <row r="2" ht="19.5" customHeight="1">
       <c r="A2" s="1" t="n">
+        <v>68</v>
+      </c>
+      <c r="B2" s="8" t="inlineStr">
+        <is>
+          <t>Deven</t>
+        </is>
+      </c>
+    </row>
+    <row r="3" ht="19.5" customHeight="1">
+      <c r="A3" s="1" t="n">
+        <v>69</v>
+      </c>
+      <c r="B3" s="8" t="inlineStr">
+        <is>
+          <t>Manraj</t>
+        </is>
+      </c>
+    </row>
+    <row r="4" ht="19.5" customHeight="1">
+      <c r="A4" s="1" t="n">
+        <v>71</v>
+      </c>
+      <c r="B4" s="8" t="inlineStr">
+        <is>
+          <t>Sakshi</t>
+        </is>
+      </c>
+    </row>
+    <row r="5" ht="18.75" customHeight="1">
+      <c r="A5" s="4" t="n">
         <v>72</v>
       </c>
-      <c r="B2" s="6" t="inlineStr">
+      <c r="B5" s="8" t="inlineStr">
         <is>
           <t>Piyush</t>
         </is>
       </c>
     </row>
-    <row r="3" ht="18.75" customHeight="1">
-      <c r="A3" s="1" t="n">
-        <v>68</v>
-      </c>
-      <c r="B3" s="6" t="inlineStr">
-        <is>
-          <t>Deven</t>
-        </is>
-      </c>
-    </row>
-    <row r="4" ht="18.75" customHeight="1">
-      <c r="A4" s="1" t="n">
-        <v>69</v>
-      </c>
-      <c r="B4" s="6" t="inlineStr">
-        <is>
-          <t>Manraj</t>
-        </is>
-      </c>
-    </row>
-    <row r="5" ht="18.75" customHeight="1">
-      <c r="A5" s="1" t="n">
-        <v>71</v>
-      </c>
-      <c r="B5" s="6" t="inlineStr">
-        <is>
-          <t>Sakshi</t>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>73</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Divyaa</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>74</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Arya</t>
         </is>
       </c>
     </row>
@@ -686,7 +771,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -694,13 +779,15 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="4" min="1" max="1"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="5" min="2" max="2"/>
-    <col hidden="1" width="13.57642857142857" bestFit="1" customWidth="1" style="5" min="3" max="3"/>
-    <col width="38.71928571428572" bestFit="1" customWidth="1" style="5" min="4" max="4"/>
-    <col hidden="1" width="13.57642857142857" bestFit="1" customWidth="1" style="5" min="5" max="5"/>
-    <col hidden="1" width="13.57642857142857" bestFit="1" customWidth="1" style="5" min="6" max="6"/>
-    <col width="31.43357142857143" bestFit="1" customWidth="1" style="6" min="7" max="7"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="6" min="1" max="1"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="2" max="2"/>
+    <col hidden="1" width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="3" max="3"/>
+    <col width="38.71928571428572" bestFit="1" customWidth="1" style="7" min="4" max="4"/>
+    <col hidden="1" width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="5" max="5"/>
+    <col hidden="1" width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="6" max="6"/>
+    <col width="31.43357142857143" bestFit="1" customWidth="1" style="8" min="7" max="7"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="8" min="8" max="8"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="8" min="9" max="9"/>
   </cols>
   <sheetData>
     <row r="1" ht="19.5" customHeight="1">
@@ -734,156 +821,295 @@
           <t>2023-04-06</t>
         </is>
       </c>
-      <c r="G1" s="6" t="inlineStr">
+      <c r="G1" s="8" t="inlineStr">
         <is>
           <t>2023-04-07</t>
+        </is>
+      </c>
+      <c r="H1" s="8" t="inlineStr">
+        <is>
+          <t>2023-04-09</t>
+        </is>
+      </c>
+      <c r="I1" s="8" t="inlineStr">
+        <is>
+          <t>2023-04-27</t>
         </is>
       </c>
     </row>
     <row r="2" ht="19.5" customHeight="1">
       <c r="A2" s="1" t="n">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>Piyush</t>
+          <t>Deven</t>
         </is>
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
-          <t>In-time: 08:52:50 Out-time: 15:03:26</t>
+          <t>In-time: 09:02:30 Out-time: 15:13:26</t>
         </is>
       </c>
       <c r="D2" s="2" t="inlineStr">
         <is>
-          <t>In-time: 08:25:46 Out-time: 14:02:52</t>
+          <t>In-time: 08:45:10 Out-time: 15:10:46</t>
         </is>
       </c>
       <c r="E2" s="2" t="inlineStr">
         <is>
-          <t>In-time: 09:52:30 Out-time: 15:10:48</t>
+          <t>In-time: 08:50:30 Out-time: 14:50:26</t>
         </is>
       </c>
       <c r="F2" s="2" t="inlineStr">
         <is>
-          <t>In-time: 08:30:50 Out-time: 15:00:26</t>
-        </is>
-      </c>
-      <c r="G2" s="6" t="inlineStr">
-        <is>
-          <t>In-time: 12:52:50 Out-time: 18:53:26</t>
+          <t>In-time: 08:32:10 Out-time: 15:05:33</t>
+        </is>
+      </c>
+      <c r="G2" s="8" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="H2" s="8" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="I2" s="8" t="inlineStr">
+        <is>
+          <t>A</t>
         </is>
       </c>
     </row>
     <row r="3" ht="19.5" customHeight="1">
       <c r="A3" s="1" t="n">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B3" s="2" t="inlineStr">
         <is>
-          <t>Deven</t>
+          <t>Manraj</t>
         </is>
       </c>
       <c r="C3" s="2" t="inlineStr">
-        <is>
-          <t>In-time: 09:02:30 Out-time: 15:13:26</t>
-        </is>
-      </c>
-      <c r="D3" s="2" t="inlineStr">
-        <is>
-          <t>In-time: 08:45:10 Out-time: 15:10:46</t>
-        </is>
-      </c>
-      <c r="E3" s="2" t="inlineStr">
-        <is>
-          <t>In-time: 08:50:30 Out-time: 14:50:26</t>
-        </is>
-      </c>
-      <c r="F3" s="2" t="inlineStr">
-        <is>
-          <t>In-time: 08:32:10 Out-time: 15:05:33</t>
-        </is>
-      </c>
-      <c r="G3" s="6" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-    </row>
-    <row r="4" ht="31.5" customHeight="1">
-      <c r="A4" s="1" t="n">
-        <v>69</v>
-      </c>
-      <c r="B4" s="2" t="inlineStr">
-        <is>
-          <t>Manraj</t>
-        </is>
-      </c>
-      <c r="C4" s="2" t="inlineStr">
         <is>
           <t>In-time: 08:46:50 
 Out-time: 14:53:26</t>
         </is>
       </c>
-      <c r="D4" s="2" t="inlineStr">
+      <c r="D3" s="2" t="inlineStr">
         <is>
           <t>In-time: 08:36:11 Out-time: 15:03:21</t>
         </is>
       </c>
-      <c r="E4" s="2" t="inlineStr">
+      <c r="E3" s="2" t="inlineStr">
         <is>
           <t>In-time: 08:58:40 
 Out-time: 14:47:05</t>
         </is>
       </c>
-      <c r="F4" s="2" t="inlineStr">
+      <c r="F3" s="2" t="inlineStr">
         <is>
           <t>In-time: 08:15:50 
 Out-time: 14:30:26</t>
         </is>
       </c>
-      <c r="G4" s="6" t="inlineStr">
+      <c r="G3" s="8" t="inlineStr">
         <is>
           <t>In-time: 18:52:50 Out-time: 18:53:26</t>
         </is>
       </c>
-    </row>
-    <row r="5" ht="19.5" customHeight="1">
-      <c r="A5" s="1" t="n">
+      <c r="H3" s="8" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="I3" s="8" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+    </row>
+    <row r="4" ht="19.5" customHeight="1">
+      <c r="A4" s="1" t="n">
         <v>71</v>
       </c>
-      <c r="B5" s="2" t="inlineStr">
+      <c r="B4" s="2" t="inlineStr">
         <is>
           <t>Sakshi</t>
         </is>
       </c>
-      <c r="C5" s="2" t="inlineStr">
+      <c r="C4" s="2" t="inlineStr">
         <is>
           <t>In-time: 08:50:45 
 Out-time: 15:05:25</t>
         </is>
       </c>
-      <c r="D5" s="2" t="inlineStr">
+      <c r="D4" s="2" t="inlineStr">
         <is>
           <t>In-time: 08:38:25 Out-time: 15:10:45</t>
         </is>
       </c>
-      <c r="E5" s="2" t="inlineStr">
+      <c r="E4" s="2" t="inlineStr">
         <is>
           <t>In-time: 08:56:15 
 Out-time: 15:10:55</t>
         </is>
       </c>
-      <c r="F5" s="2" t="inlineStr">
+      <c r="F4" s="2" t="inlineStr">
         <is>
           <t>In-time: 09:00:45 
 Out-time: 15:52:25</t>
         </is>
       </c>
-      <c r="G5" s="6" t="inlineStr">
-        <is>
-          <t>In-time: 19:56:29 
-Out-time: 19:59:08</t>
+      <c r="G4" s="8" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="H4" s="8" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="I4" s="8" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+    </row>
+    <row r="5" ht="18.75" customHeight="1">
+      <c r="A5" s="4" t="n">
+        <v>72</v>
+      </c>
+      <c r="B5" s="7" t="inlineStr">
+        <is>
+          <t>Piyush</t>
+        </is>
+      </c>
+      <c r="C5" s="7" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="D5" s="7" t="inlineStr">
+        <is>
+          <t>In-time: 09:17:21 Out-time: 15:16:55</t>
+        </is>
+      </c>
+      <c r="E5" s="7" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="F5" s="7" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="G5" s="8" t="inlineStr">
+        <is>
+          <t>In-time: 08:14:58 Out-time: 14:52:55</t>
+        </is>
+      </c>
+      <c r="H5" s="8" t="inlineStr">
+        <is>
+          <t>In-time: 08:25:28 Out-time: 15:11:12</t>
+        </is>
+      </c>
+      <c r="I5" s="8" t="inlineStr">
+        <is>
+          <t>In-time: 09:17:28 Out-time: 13:18:55</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>73</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Divyaa</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>74</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Arya</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>A</t>
         </is>
       </c>
     </row>

</xml_diff>